<commit_message>
Working [Edit] (Saving, NO RELATIONS yET)
</commit_message>
<xml_diff>
--- a/formato metadatos.xlsx
+++ b/formato metadatos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lección" sheetId="11" r:id="rId1"/>
@@ -1541,7 +1541,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="52">
   <si>
     <t>Título</t>
   </si>
@@ -2506,6 +2506,21 @@
   </si>
   <si>
     <t>obj1</t>
+  </si>
+  <si>
+    <t>el baile de william</t>
+  </si>
+  <si>
+    <t>music, play, magazines and more</t>
+  </si>
+  <si>
+    <t>q3qwewe</t>
+  </si>
+  <si>
+    <t>qweqweqweqw123123123</t>
+  </si>
+  <si>
+    <t>eqweqwe2312312edfghjkyiutyrtredscvbnhjgyt</t>
   </si>
 </sst>
 </file>
@@ -3300,8 +3315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3342,7 +3357,9 @@
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="27" t="s">
+        <v>47</v>
+      </c>
       <c r="C4" s="26"/>
     </row>
     <row r="5" spans="1:3" ht="129" customHeight="1" x14ac:dyDescent="0.25">
@@ -3358,28 +3375,36 @@
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="23"/>
+      <c r="B6" s="23" t="s">
+        <v>48</v>
+      </c>
       <c r="C6" s="24"/>
     </row>
     <row r="7" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="29"/>
+      <c r="B7" s="29" t="s">
+        <v>49</v>
+      </c>
       <c r="C7" s="30"/>
     </row>
     <row r="8" spans="1:3" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="23" t="s">
+        <v>50</v>
+      </c>
       <c r="C8" s="24"/>
     </row>
     <row r="9" spans="1:3" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="C9" s="24"/>
     </row>
     <row r="10" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3418,8 +3443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>